<commit_message>
richards: theis 2phase version tested and doco
r24161
</commit_message>
<xml_diff>
--- a/modules/combined/doc/richards/tests/data/th.xlsx
+++ b/modules/combined/doc/richards/tests/data/th.xlsx
@@ -10,9 +10,11 @@
     <sheet name="theis_comparison" sheetId="6" r:id="rId1"/>
     <sheet name="expected" sheetId="5" r:id="rId2"/>
     <sheet name="th01" sheetId="3" r:id="rId3"/>
+    <sheet name="th21" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="th01_" localSheetId="2">'th01'!$C$3:$E$85</definedName>
+    <definedName name="th21_" localSheetId="3">'th21'!$C$3:$E$32</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -29,11 +31,20 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="th21" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\tests\richards\theis\th21.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Perm=</t>
   </si>
@@ -120,6 +131,9 @@
   </si>
   <si>
     <t>flow rate</t>
+  </si>
+  <si>
+    <t>drawdown(m)</t>
   </si>
 </sst>
 </file>
@@ -230,9 +244,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12930796150481189"/>
-          <c:y val="4.2908288637833344E-2"/>
+          <c:y val="4.2908288637833351E-2"/>
           <c:w val="0.80551837270341198"/>
-          <c:h val="0.74960995093004712"/>
+          <c:h val="0.74960995093004723"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2058,11 +2072,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="170433920"/>
-        <c:axId val="170998784"/>
+        <c:axId val="130032768"/>
+        <c:axId val="130034688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170433920"/>
+        <c:axId val="130032768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2095,12 +2109,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170998784"/>
+        <c:crossAx val="130034688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170998784"/>
+        <c:axId val="130034688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2132,7 +2146,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170433920"/>
+        <c:crossAx val="130032768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2187,6 +2201,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="th01" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="th21" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2658,15 +2676,15 @@
         <v>0.2</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:D19" si="0">$D$13/B16</f>
+        <f t="shared" ref="D16" si="0">$D$13/B16</f>
         <v>1.5625000000000029</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" ref="F16:F19" si="1">-0.577216-LN(D16)+D16-D16^2/2/FACT(2)+D16^3/3/FACT(3)-D16^4/4/FACT(4)+D16^5/5/FACT(5)-D16^6/6/FACT(6)+D16^7/7/FACT(7)-D16^8/8/FACT(8)+D16^9/9/FACT(9)-D16^10/10/FACT(10)+D16^11/11/FACT(11)</f>
+        <f t="shared" ref="F16" si="1">-0.577216-LN(D16)+D16-D16^2/2/FACT(2)+D16^3/3/FACT(3)-D16^4/4/FACT(4)+D16^5/5/FACT(5)-D16^6/6/FACT(6)+D16^7/7/FACT(7)-D16^8/8/FACT(8)+D16^9/9/FACT(9)-D16^10/10/FACT(10)+D16^11/11/FACT(11)</f>
         <v>9.1187590679529432E-2</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H19" si="2">$D$1/4/PI()/$D$8*F16</f>
+        <f t="shared" ref="H16" si="2">$D$1/4/PI()/$D$8*F16</f>
         <v>7.2564779026437765E-2</v>
       </c>
     </row>
@@ -6241,7 +6259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:I202"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G85"/>
     </sheetView>
   </sheetViews>
@@ -8435,4 +8453,471 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+      <c r="G4">
+        <f>($E$4-E4)/10000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>96926.490096177004</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G32" si="0">($E$4-E5)/10000</f>
+        <v>0.30735099038229963</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>93815.261885077998</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.61847381149220015</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>89603.213155149002</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.0396786844850998</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
+      <c r="C8">
+        <v>3.1111111111111001</v>
+      </c>
+      <c r="D8">
+        <v>222.22222222222001</v>
+      </c>
+      <c r="E8">
+        <v>86416.480563721998</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.3583519436278002</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9">
+        <v>4.3456790123457001</v>
+      </c>
+      <c r="D9">
+        <v>246.91358024690999</v>
+      </c>
+      <c r="E9">
+        <v>83869.417534288994</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1.6130582465711005</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10">
+        <v>5.7174211248285003</v>
+      </c>
+      <c r="D10">
+        <v>274.34842249656998</v>
+      </c>
+      <c r="E10">
+        <v>81733.073669877005</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.8266926330122994</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11">
+        <v>7.2415790275873002</v>
+      </c>
+      <c r="D11">
+        <v>304.83158055174999</v>
+      </c>
+      <c r="E11">
+        <v>79875.208744575997</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.0124791255424004</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12">
+        <v>8.9350878084302998</v>
+      </c>
+      <c r="D12">
+        <v>338.70175616861002</v>
+      </c>
+      <c r="E12">
+        <v>78215.705321353002</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.1784294678646998</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>212.98243831394001</v>
+      </c>
+      <c r="E13">
+        <v>77294.658842735007</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2.2705341157264991</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14">
+        <v>75859.211112684003</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.4140788887315998</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15">
+        <v>14.177777777777999</v>
+      </c>
+      <c r="D15">
+        <v>435.55555555555998</v>
+      </c>
+      <c r="E15">
+        <v>74541.813191239999</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.5458186808760002</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16">
+        <v>16.549135802468999</v>
+      </c>
+      <c r="D16">
+        <v>474.27160493827</v>
+      </c>
+      <c r="E16">
+        <v>73317.705670737996</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2.6682294329262004</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17">
+        <v>19.131281207133</v>
+      </c>
+      <c r="D17">
+        <v>516.42908093278004</v>
+      </c>
+      <c r="E17">
+        <v>72168.835078931006</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>2.7831164921068994</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18">
+        <v>21.942950647766999</v>
+      </c>
+      <c r="D18">
+        <v>562.33388812681005</v>
+      </c>
+      <c r="E18">
+        <v>71081.667505474994</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2.8918332494525005</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19">
+        <v>25.004546260902</v>
+      </c>
+      <c r="D19">
+        <v>612.31912262697006</v>
+      </c>
+      <c r="E19">
+        <v>70045.816817244006</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2.9954183182755996</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20">
+        <v>28.338283706315</v>
+      </c>
+      <c r="D20">
+        <v>666.74748908269999</v>
+      </c>
+      <c r="E20">
+        <v>69053.151900298006</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>3.0946848099701993</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21">
+        <v>31.968353369098999</v>
+      </c>
+      <c r="D21">
+        <v>726.01393255671996</v>
+      </c>
+      <c r="E21">
+        <v>68097.196939280999</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>3.1902803060719003</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22">
+        <v>35.921095890796998</v>
+      </c>
+      <c r="D22">
+        <v>790.54850433954005</v>
+      </c>
+      <c r="E22">
+        <v>67172.717255156997</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>3.2827282744843003</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23">
+        <v>40.225193303311997</v>
+      </c>
+      <c r="D23">
+        <v>860.81948250305004</v>
+      </c>
+      <c r="E23">
+        <v>66275.426258766005</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>3.3724573741233996</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24">
+        <v>44.911877152495002</v>
+      </c>
+      <c r="D24">
+        <v>937.33676983665998</v>
+      </c>
+      <c r="E24">
+        <v>65401.773609532</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3.4598226390467999</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25">
+        <v>50.015155121606</v>
+      </c>
+      <c r="D25">
+        <v>1020.6555938220999</v>
+      </c>
+      <c r="E25">
+        <v>64548.789131696001</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3.5451210868303997</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26">
+        <v>55.572057799082003</v>
+      </c>
+      <c r="D26">
+        <v>1111.3805354952001</v>
+      </c>
+      <c r="E26">
+        <v>63713.965833239003</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>3.6286034166760999</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27">
+        <v>61.622907381223001</v>
+      </c>
+      <c r="D27">
+        <v>1210.1699164280999</v>
+      </c>
+      <c r="E27">
+        <v>62895.170875837</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>3.7104829124163001</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28">
+        <v>68.211610259554007</v>
+      </c>
+      <c r="D28">
+        <v>1317.7405756661999</v>
+      </c>
+      <c r="E28">
+        <v>62090.576881382003</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>3.7909423118617998</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29">
+        <v>75.385975615958003</v>
+      </c>
+      <c r="D29">
+        <v>1434.873071281</v>
+      </c>
+      <c r="E29">
+        <v>61298.608245967996</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>3.8701391754032004</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30">
+        <v>83.198062337376996</v>
+      </c>
+      <c r="D30">
+        <v>1562.4173442837</v>
+      </c>
+      <c r="E30">
+        <v>60517.898709036002</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>3.9482101290963998</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31">
+        <v>91.704556767366</v>
+      </c>
+      <c r="D31">
+        <v>1701.2988859978</v>
+      </c>
+      <c r="E31">
+        <v>59747.257458179003</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>4.0252742541820998</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>1659.0886465267999</v>
+      </c>
+      <c r="E32">
+        <v>59059.009472284997</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>4.0940990527715</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>